<commit_message>
prep interview 230322 at work
</commit_message>
<xml_diff>
--- a/1. Personal/3. IN/02. SS/Job description_AP SW개발팀_analysis.xlsx
+++ b/1. Personal/3. IN/02. SS/Job description_AP SW개발팀_analysis.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/840367323e0d0e2d/Documents/Taeho/blog/nacl1119.github.io/1. Personal/3. IN/02. SS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\project\programming\nacl1119.github.io\1. Personal\3. IN\02. SS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{DE9D45EC-96F9-4781-B3BD-3629ADE0C3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8BB2810-E315-4E57-BDFC-F4B497432AB0}"/>
   <bookViews>
-    <workbookView xWindow="28665" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28670" yWindow="-140" windowWidth="29070" windowHeight="15750"/>
   </bookViews>
   <sheets>
     <sheet name="Job Description" sheetId="6" r:id="rId1"/>
@@ -2026,7 +2025,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2221,7 +2220,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2502,25 +2501,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" customWidth="1"/>
-    <col min="2" max="2" width="27.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.69921875" customWidth="1"/>
-    <col min="4" max="4" width="47.19921875" customWidth="1"/>
+    <col min="1" max="1" width="3.4140625" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.6640625" customWidth="1"/>
+    <col min="4" max="4" width="47.1640625" customWidth="1"/>
     <col min="5" max="5" width="57.5" customWidth="1"/>
-    <col min="6" max="6" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2537,7 +2536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="254.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:6" ht="254.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="17" t="s">
         <v>11</v>
       </c>
@@ -2554,7 +2553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="187.2" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="176" x14ac:dyDescent="0.45">
       <c r="B4" s="8"/>
       <c r="C4" s="9" t="s">
         <v>49</v>
@@ -2567,7 +2566,7 @@
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="2:6" ht="343.2" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" ht="352" x14ac:dyDescent="0.45">
       <c r="B5" s="17" t="s">
         <v>12</v>
       </c>
@@ -2584,7 +2583,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="62.4" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:6" ht="64" x14ac:dyDescent="0.45">
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>70</v>
@@ -2595,61 +2594,61 @@
       <c r="E6" s="5"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="2:6" ht="187.2" x14ac:dyDescent="0.4">
-      <c r="B7" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="24" t="s">
+    <row r="7" spans="2:6" ht="192" x14ac:dyDescent="0.45">
+      <c r="B7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="31.2" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:6" ht="136" x14ac:dyDescent="0.45">
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="16"/>
+      <c r="E8" s="15" t="s">
+        <v>59</v>
+      </c>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="2:6" ht="187.2" x14ac:dyDescent="0.4">
-      <c r="B9" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="20" t="s">
+    <row r="9" spans="2:6" ht="192" x14ac:dyDescent="0.45">
+      <c r="B9" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="121.8" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:6" ht="32" x14ac:dyDescent="0.45">
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="15" t="s">
-        <v>59</v>
-      </c>
+      <c r="E10" s="16"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="2:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
@@ -2666,7 +2665,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="31.2" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:6" ht="32" x14ac:dyDescent="0.45">
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
         <v>51</v>
@@ -2675,7 +2674,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="2:6" ht="181.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:6" ht="181.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="14" t="s">
         <v>13</v>
       </c>
@@ -2692,7 +2691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B14" s="14"/>
       <c r="C14" s="11" t="s">
         <v>74</v>
@@ -2701,7 +2700,7 @@
       <c r="E14" s="12"/>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="2:6" ht="392.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:6" ht="392.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="14" t="s">
         <v>14</v>
       </c>
@@ -2718,7 +2717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:6" ht="48" x14ac:dyDescent="0.45">
       <c r="B16" s="14"/>
       <c r="C16" s="11" t="s">
         <v>79</v>
@@ -2727,7 +2726,7 @@
       <c r="E16" s="11"/>
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="2:6" ht="228.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:6" ht="228.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="14" t="s">
         <v>20</v>
       </c>
@@ -2744,7 +2743,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B18" s="14" t="s">
         <v>63</v>
       </c>
@@ -2753,7 +2752,7 @@
       <c r="E18" s="11"/>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="2:6" ht="198.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:6" ht="198.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="14" t="s">
         <v>38</v>
       </c>
@@ -2770,7 +2769,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B20" s="14"/>
       <c r="C20" s="11" t="s">
         <v>48</v>
@@ -2779,7 +2778,7 @@
       <c r="E20" s="12"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="2:6" ht="202.8" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:6" ht="208" x14ac:dyDescent="0.45">
       <c r="B21" s="14" t="s">
         <v>8</v>
       </c>
@@ -2796,7 +2795,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="262.2" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:6" ht="262.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="14" t="s">
         <v>9</v>
       </c>
@@ -2813,7 +2812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="109.2" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:6" ht="112" x14ac:dyDescent="0.45">
       <c r="B23" s="14" t="s">
         <v>10</v>
       </c>
@@ -2830,7 +2829,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24" s="14"/>
       <c r="C24" s="11" t="s">
         <v>60</v>
@@ -2839,7 +2838,7 @@
       <c r="E24" s="12"/>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="2:6" ht="328.2" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:6" ht="328.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="14" t="s">
         <v>21</v>
       </c>
@@ -2856,7 +2855,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:6" ht="48" x14ac:dyDescent="0.45">
       <c r="B26" s="14"/>
       <c r="C26" s="12" t="s">
         <v>57</v>
@@ -2867,7 +2866,7 @@
       <c r="E26" s="12"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="2:6" ht="140.4" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:6" ht="144" x14ac:dyDescent="0.45">
       <c r="B27" s="10" t="s">
         <v>19</v>
       </c>
@@ -2884,7 +2883,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="156" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:6" ht="160" x14ac:dyDescent="0.45">
       <c r="B28" s="10" t="s">
         <v>22</v>
       </c>

</xml_diff>